<commit_message>
Fixed retirees to hit oldplan benefit levels
</commit_message>
<xml_diff>
--- a/data-raw/PrototypeAnalysis(13).xlsx
+++ b/data-raw/PrototypeAnalysis(13).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13335" tabRatio="789" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13335" tabRatio="789" firstSheet="4" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="34" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="350">
   <si>
     <t>CRR locations for CAFRs and AVs</t>
   </si>
@@ -888,9 +888,6 @@
     <t xml:space="preserve">For each prototype, we </t>
   </si>
   <si>
-    <t>young</t>
-  </si>
-  <si>
     <t>prototype</t>
   </si>
   <si>
@@ -1213,6 +1210,15 @@
   </si>
   <si>
     <t>30+</t>
+  </si>
+  <si>
+    <t>highabratio</t>
+  </si>
+  <si>
+    <t>St-Paul's total</t>
+  </si>
+  <si>
+    <t>A adjust the average benefit to equal MI-MPSERS benefit</t>
   </si>
 </sst>
 </file>
@@ -2845,7 +2851,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2883,7 +2889,7 @@
         <v>49</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2923,7 +2929,7 @@
         <v>107</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2931,7 +2937,7 @@
         <v>108</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2939,7 +2945,7 @@
         <v>109</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2947,7 +2953,7 @@
         <v>228</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2955,7 +2961,7 @@
         <v>230</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2963,7 +2969,7 @@
         <v>231</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2984,7 +2990,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>226</v>
@@ -2992,7 +2998,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>229</v>
@@ -3000,7 +3006,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>227</v>
@@ -3008,15 +3014,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>127</v>
@@ -3024,7 +3030,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>128</v>
@@ -3032,7 +3038,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>129</v>
@@ -3040,7 +3046,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>110</v>
@@ -3094,12 +3100,12 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -3119,10 +3125,10 @@
         <v>4</v>
       </c>
       <c r="K3" t="s">
+        <v>310</v>
+      </c>
+      <c r="L3" t="s">
         <v>311</v>
-      </c>
-      <c r="L3" t="s">
-        <v>312</v>
       </c>
       <c r="M3" t="s">
         <v>55</v>
@@ -3140,7 +3146,7 @@
         <v>59</v>
       </c>
       <c r="R3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -3210,7 +3216,7 @@
         <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3502,7 +3508,7 @@
         <v>1117</v>
       </c>
       <c r="K10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -4502,7 +4508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
@@ -4518,27 +4524,27 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -4826,7 +4832,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B39" s="28">
         <v>0</v>
@@ -4846,9 +4852,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:P160"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4863,7 +4867,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -4874,7 +4878,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E2" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -4885,45 +4889,45 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E3" t="s">
         <v>275</v>
       </c>
-      <c r="E3" t="s">
+      <c r="L3" t="s">
         <v>276</v>
-      </c>
-      <c r="L3" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
+        <v>277</v>
+      </c>
+      <c r="F4" t="s">
         <v>278</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>279</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>280</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>281</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>282</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>283</v>
       </c>
-      <c r="K4" t="s">
-        <v>284</v>
-      </c>
       <c r="M4" t="s">
+        <v>293</v>
+      </c>
+      <c r="N4" t="s">
         <v>294</v>
       </c>
-      <c r="N4" t="s">
-        <v>295</v>
-      </c>
       <c r="P4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -4975,7 +4979,7 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E6" s="14">
         <v>318</v>
@@ -5011,7 +5015,7 @@
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E7" s="14">
         <v>6493</v>
@@ -5049,7 +5053,7 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E8" s="14">
         <v>11974</v>
@@ -5089,7 +5093,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E9" s="14">
         <v>8672</v>
@@ -5131,7 +5135,7 @@
         <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E10" s="14">
         <v>7759</v>
@@ -5175,7 +5179,7 @@
         <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E11" s="14">
         <v>9398</v>
@@ -5221,7 +5225,7 @@
         <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E12" s="14">
         <v>8862</v>
@@ -5269,7 +5273,7 @@
         <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E13" s="14">
         <v>7010</v>
@@ -5317,7 +5321,7 @@
         <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E14" s="14">
         <v>5382</v>
@@ -5365,7 +5369,7 @@
         <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E15" s="14">
         <v>3178</v>
@@ -5413,7 +5417,7 @@
         <v>67</v>
       </c>
       <c r="D16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E16" s="14">
         <v>1525</v>
@@ -5557,7 +5561,7 @@
         <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E19" s="32">
         <f>+E50/$M65</f>
@@ -5607,7 +5611,7 @@
         <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E20" s="32">
         <f t="shared" ref="E20:K20" si="2">+E51/$M66</f>
@@ -5653,7 +5657,7 @@
         <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E21" s="32">
         <f t="shared" ref="E21:K21" si="4">+E52/$M67</f>
@@ -5699,7 +5703,7 @@
         <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E22" s="32">
         <f t="shared" ref="E22:K22" si="5">+E53/$M68</f>
@@ -5745,7 +5749,7 @@
         <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E23" s="32">
         <f t="shared" ref="E23:K23" si="6">+E54/$M69</f>
@@ -5791,7 +5795,7 @@
         <v>42</v>
       </c>
       <c r="D24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E24" s="32">
         <f t="shared" ref="E24:K24" si="7">+E55/$M70</f>
@@ -5837,7 +5841,7 @@
         <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E25" s="32">
         <f t="shared" ref="E25:K25" si="8">+E56/$M71</f>
@@ -5883,7 +5887,7 @@
         <v>52</v>
       </c>
       <c r="D26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E26" s="32">
         <f t="shared" ref="E26:K26" si="9">+E57/$M72</f>
@@ -5929,7 +5933,7 @@
         <v>57</v>
       </c>
       <c r="D27" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E27" s="32">
         <f t="shared" ref="E27:K27" si="10">+E58/$M73</f>
@@ -5975,7 +5979,7 @@
         <v>62</v>
       </c>
       <c r="D28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E28" s="32">
         <f t="shared" ref="E28:K28" si="11">+E59/$M74</f>
@@ -6021,7 +6025,7 @@
         <v>67</v>
       </c>
       <c r="D29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E29" s="32">
         <f t="shared" ref="E29:K29" si="12">+E60/$M75</f>
@@ -6118,13 +6122,13 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
+        <v>300</v>
+      </c>
+      <c r="L33" t="s">
         <v>301</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>302</v>
-      </c>
-      <c r="M33" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -6704,18 +6708,18 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M49" t="s">
+        <v>296</v>
+      </c>
+      <c r="N49" t="s">
         <v>297</v>
-      </c>
-      <c r="N49" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -7198,13 +7202,13 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L64" t="s">
+        <v>298</v>
+      </c>
+      <c r="M64" t="s">
         <v>299</v>
-      </c>
-      <c r="M64" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -7795,21 +7799,21 @@
     </row>
     <row r="83" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D85" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E85" t="s">
+        <v>309</v>
+      </c>
+      <c r="F85" t="s">
         <v>310</v>
       </c>
-      <c r="F85" t="s">
+      <c r="G85" t="s">
         <v>311</v>
-      </c>
-      <c r="G85" t="s">
-        <v>312</v>
       </c>
       <c r="H85" t="s">
         <v>55</v>
@@ -7824,10 +7828,10 @@
         <v>58</v>
       </c>
       <c r="L85" t="s">
+        <v>312</v>
+      </c>
+      <c r="M85" t="s">
         <v>313</v>
-      </c>
-      <c r="M85" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -7882,7 +7886,7 @@
         <v>22</v>
       </c>
       <c r="D87" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E87" s="14">
         <v>27192</v>
@@ -8251,7 +8255,7 @@
         <v>67</v>
       </c>
       <c r="D96" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E96" s="14">
         <v>13249</v>
@@ -8292,7 +8296,7 @@
         <v>117</v>
       </c>
       <c r="D97" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E97" s="14">
         <v>37720</v>
@@ -8324,7 +8328,7 @@
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D99" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
@@ -8332,7 +8336,7 @@
         <v>20</v>
       </c>
       <c r="D100" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E100" s="33">
         <f>+E101</f>
@@ -8885,7 +8889,7 @@
         <v>70</v>
       </c>
       <c r="D111" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E111" s="15">
         <f>+E110</f>
@@ -8929,7 +8933,7 @@
     </row>
     <row r="118" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
@@ -10002,7 +10006,7 @@
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
@@ -10634,8 +10638,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10645,17 +10649,22 @@
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>122</v>
       </c>
@@ -10671,8 +10680,11 @@
       <c r="E4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -10683,13 +10695,16 @@
         <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E5" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -10705,8 +10720,11 @@
       <c r="E6" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -10722,8 +10740,11 @@
       <c r="E7" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -10739,8 +10760,11 @@
       <c r="E8" s="14">
         <v>124</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="14">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -10756,8 +10780,11 @@
       <c r="E9" s="14">
         <v>543</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="14">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -10773,8 +10800,11 @@
       <c r="E10" s="14">
         <v>856</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="14">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -10790,8 +10820,11 @@
       <c r="E11" s="14">
         <v>589</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="14">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -10807,8 +10840,11 @@
       <c r="E12" s="14">
         <v>417</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="14">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -10824,8 +10860,11 @@
       <c r="E13" s="14">
         <v>295</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="14">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -10841,8 +10880,11 @@
       <c r="E14" s="14">
         <v>159</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="14">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -10853,13 +10895,16 @@
         <v>92</v>
       </c>
       <c r="D15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E15" s="14">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="14">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -10870,9 +10915,12 @@
         <v>117</v>
       </c>
       <c r="D16" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E16" s="14">
+        <v>3047</v>
+      </c>
+      <c r="F16" s="14">
         <v>3047</v>
       </c>
     </row>
@@ -10887,12 +10935,15 @@
         <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E17" s="14">
-        <v>0</v>
-      </c>
-      <c r="F17" s="25"/>
+        <f t="shared" ref="E17:E27" si="0">+F17*21022/31144</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -10908,9 +10959,12 @@
         <v>63</v>
       </c>
       <c r="E18" s="14">
-        <v>0</v>
-      </c>
-      <c r="F18" s="25"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -10926,9 +10980,12 @@
         <v>64</v>
       </c>
       <c r="E19" s="14">
+        <f t="shared" si="0"/>
+        <v>1059.0649242229642</v>
+      </c>
+      <c r="F19" s="14">
         <v>1569</v>
       </c>
-      <c r="F19" s="25"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -10944,9 +11001,12 @@
         <v>65</v>
       </c>
       <c r="E20" s="14">
+        <f t="shared" si="0"/>
+        <v>15943.348317492935</v>
+      </c>
+      <c r="F20" s="14">
         <v>23620</v>
       </c>
-      <c r="F20" s="25"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -10962,9 +11022,12 @@
         <v>66</v>
       </c>
       <c r="E21" s="14">
+        <f t="shared" si="0"/>
+        <v>18703.397058823528</v>
+      </c>
+      <c r="F21" s="14">
         <v>27709</v>
       </c>
-      <c r="F21" s="25"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -10980,9 +11043,12 @@
         <v>71</v>
       </c>
       <c r="E22" s="14">
+        <f t="shared" si="0"/>
+        <v>20076.333996917543</v>
+      </c>
+      <c r="F22" s="14">
         <v>29743</v>
       </c>
-      <c r="F22" s="25"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -10998,9 +11064,12 @@
         <v>72</v>
       </c>
       <c r="E23" s="14">
+        <f t="shared" si="0"/>
+        <v>20372.656177754943</v>
+      </c>
+      <c r="F23" s="14">
         <v>30182</v>
       </c>
-      <c r="F23" s="25"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -11016,9 +11085,12 @@
         <v>73</v>
       </c>
       <c r="E24" s="14">
+        <f t="shared" si="0"/>
+        <v>24429.367582840998</v>
+      </c>
+      <c r="F24" s="14">
         <v>36192</v>
       </c>
-      <c r="F24" s="25"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -11034,9 +11106,12 @@
         <v>74</v>
       </c>
       <c r="E25" s="14">
+        <f t="shared" si="0"/>
+        <v>27107.067107629078</v>
+      </c>
+      <c r="F25" s="14">
         <v>40159</v>
       </c>
-      <c r="F25" s="25"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -11052,9 +11127,12 @@
         <v>75</v>
       </c>
       <c r="E26" s="14">
+        <f t="shared" si="0"/>
+        <v>20976.100436681223</v>
+      </c>
+      <c r="F26" s="14">
         <v>31076</v>
       </c>
-      <c r="F26" s="25"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -11067,12 +11145,15 @@
         <v>92</v>
       </c>
       <c r="D27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E27" s="14">
+        <f t="shared" si="0"/>
+        <v>19289.291484716156</v>
+      </c>
+      <c r="F27" s="14">
         <v>28577</v>
       </c>
-      <c r="F27" s="25"/>
       <c r="G27" s="25"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -11086,12 +11167,15 @@
         <v>117</v>
       </c>
       <c r="D28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E28" s="14">
+        <f>+F28*21022/31144</f>
+        <v>21022</v>
+      </c>
+      <c r="F28" s="14">
         <v>31144</v>
       </c>
-      <c r="F28" s="25"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E29" s="14"/>
@@ -16133,9 +16217,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16182,21 +16264,21 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -16204,10 +16286,10 @@
         <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -16215,99 +16297,99 @@
         <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>240</v>
+        <v>347</v>
       </c>
       <c r="B17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B18" t="s">
+        <v>258</v>
+      </c>
+      <c r="C18" t="s">
         <v>259</v>
       </c>
-      <c r="C18" t="s">
-        <v>260</v>
-      </c>
       <c r="D18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>305</v>
+      </c>
+      <c r="B19" t="s">
+        <v>308</v>
+      </c>
+      <c r="C19" t="s">
+        <v>307</v>
+      </c>
+      <c r="D19" t="s">
         <v>306</v>
-      </c>
-      <c r="B19" t="s">
-        <v>309</v>
-      </c>
-      <c r="C19" t="s">
-        <v>308</v>
-      </c>
-      <c r="D19" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -21965,7 +22047,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E2" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -21985,10 +22067,10 @@
         <v>4</v>
       </c>
       <c r="J4" t="s">
+        <v>310</v>
+      </c>
+      <c r="K4" t="s">
         <v>311</v>
-      </c>
-      <c r="K4" t="s">
-        <v>312</v>
       </c>
       <c r="L4" t="s">
         <v>55</v>
@@ -22006,7 +22088,7 @@
         <v>59</v>
       </c>
       <c r="Q4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="R4" t="s">
         <v>61</v>
@@ -22068,7 +22150,7 @@
         <v>117</v>
       </c>
       <c r="S5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>